<commit_message>
Updated with round of fixes (3 errors remaining)
</commit_message>
<xml_diff>
--- a/2021/combined_strategic_authorities.xlsx
+++ b/2021/combined_strategic_authorities.xlsx
@@ -753,7 +753,7 @@
         <v>0.2</v>
       </c>
       <c r="H5">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="I5">
         <v>0.6</v>
@@ -771,7 +771,7 @@
         <v>0.5</v>
       </c>
       <c r="N5">
-        <v>0.4617857142857144</v>
+        <v>0.4767857142857143</v>
       </c>
       <c r="Q5" t="s">
         <v>46</v>
@@ -791,7 +791,7 @@
         <v>37</v>
       </c>
       <c r="E6">
-        <v>0.4761904761904762</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="F6">
         <v>0.2777777777777778</v>
@@ -818,7 +818,7 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.3605952380952381</v>
+        <v>0.353452380952381</v>
       </c>
       <c r="Q6" t="s">
         <v>47</v>
@@ -909,10 +909,10 @@
         <v>0.2</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8">
-        <v>0.3036904761904762</v>
+        <v>0.2536904761904762</v>
       </c>
       <c r="Q8" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Removed 1 deleted question
Tidied up questions.csv to exclude deleted qs for clarity
</commit_message>
<xml_diff>
--- a/2021/combined_strategic_authorities.xlsx
+++ b/2021/combined_strategic_authorities.xlsx
@@ -612,7 +612,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>0.9</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="I2">
         <v>0.8</v>
@@ -630,7 +630,7 @@
         <v>1</v>
       </c>
       <c r="N2">
-        <v>0.8952380952380954</v>
+        <v>0.8935714285714287</v>
       </c>
       <c r="Q2" t="s">
         <v>44</v>
@@ -659,7 +659,7 @@
         <v>0.5714285714285714</v>
       </c>
       <c r="H3">
-        <v>0.8</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="I3">
         <v>0.6</v>
@@ -677,7 +677,7 @@
         <v>0.75</v>
       </c>
       <c r="N3">
-        <v>0.6174999999999999</v>
+        <v>0.6141666666666666</v>
       </c>
       <c r="Q3" t="s">
         <v>45</v>
@@ -706,7 +706,7 @@
         <v>0.4</v>
       </c>
       <c r="H4">
-        <v>0.7</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="I4">
         <v>0.8</v>
@@ -724,7 +724,7 @@
         <v>0.75</v>
       </c>
       <c r="N4">
-        <v>0.5803571428571429</v>
+        <v>0.5753571428571428</v>
       </c>
       <c r="Q4" t="s">
         <v>46</v>
@@ -753,7 +753,7 @@
         <v>0.2</v>
       </c>
       <c r="H5">
-        <v>0.4</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="I5">
         <v>0.6</v>
@@ -771,7 +771,7 @@
         <v>0.5</v>
       </c>
       <c r="N5">
-        <v>0.4767857142857143</v>
+        <v>0.4667857142857144</v>
       </c>
       <c r="Q5" t="s">
         <v>46</v>
@@ -800,7 +800,7 @@
         <v>0.4</v>
       </c>
       <c r="H6">
-        <v>0.5</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="I6">
         <v>0.8</v>
@@ -818,7 +818,7 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.353452380952381</v>
+        <v>0.3451190476190477</v>
       </c>
       <c r="Q6" t="s">
         <v>47</v>
@@ -847,7 +847,7 @@
         <v>0.4</v>
       </c>
       <c r="H7">
-        <v>0.4</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="I7">
         <v>0.2</v>
@@ -865,7 +865,7 @@
         <v>0.5</v>
       </c>
       <c r="N7">
-        <v>0.3197619047619048</v>
+        <v>0.3097619047619048</v>
       </c>
       <c r="Q7" t="s">
         <v>48</v>
@@ -894,7 +894,7 @@
         <v>0.2</v>
       </c>
       <c r="H8">
-        <v>0.5</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="I8">
         <v>0.4</v>
@@ -912,7 +912,7 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <v>0.2536904761904762</v>
+        <v>0.2620238095238095</v>
       </c>
       <c r="Q8" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Fix regression where four plans excluded
</commit_message>
<xml_diff>
--- a/2021/combined_strategic_authorities.xlsx
+++ b/2021/combined_strategic_authorities.xlsx
@@ -97,6 +97,9 @@
     <t>West Yorkshire Combined Authority</t>
   </si>
   <si>
+    <t>North of Tyne Combined Authority</t>
+  </si>
+  <si>
     <t>West of England Combined Authority</t>
   </si>
   <si>
@@ -109,9 +112,6 @@
     <t>Cambridgeshire and Peterborough Combined Authority</t>
   </si>
   <si>
-    <t>North of Tyne Combined Authority</t>
-  </si>
-  <si>
     <t>North East Combined Authority</t>
   </si>
   <si>
@@ -130,6 +130,9 @@
     <t>WYCA</t>
   </si>
   <si>
+    <t>NTCA</t>
+  </si>
+  <si>
     <t>WECA</t>
   </si>
   <si>
@@ -142,9 +145,6 @@
     <t>CPCA</t>
   </si>
   <si>
-    <t>NTCA</t>
-  </si>
-  <si>
     <t>NECA</t>
   </si>
   <si>
@@ -160,10 +160,10 @@
     <t>Yorkshire and The Humber</t>
   </si>
   <si>
+    <t>North East</t>
+  </si>
+  <si>
     <t>South West</t>
-  </si>
-  <si>
-    <t>North East</t>
   </si>
   <si>
     <t>East</t>
@@ -838,34 +838,34 @@
         <v>38</v>
       </c>
       <c r="E7">
-        <v>0.4761904761904762</v>
+        <v>0.3809523809523809</v>
       </c>
       <c r="F7">
-        <v>0.3888888888888889</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="G7">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="H7">
         <v>0.3333333333333333</v>
       </c>
       <c r="I7">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="J7">
         <v>0.5</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="M7">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="N7">
-        <v>0.3097619047619048</v>
+        <v>0.3271428571428571</v>
       </c>
       <c r="Q7" t="s">
         <v>48</v>
@@ -885,37 +885,37 @@
         <v>39</v>
       </c>
       <c r="E8">
-        <v>0.2857142857142857</v>
+        <v>0.4761904761904762</v>
       </c>
       <c r="F8">
-        <v>0.05555555555555555</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="G8">
+        <v>0.4</v>
+      </c>
+      <c r="H8">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="I8">
         <v>0.2</v>
       </c>
-      <c r="H8">
-        <v>0.5555555555555556</v>
-      </c>
-      <c r="I8">
-        <v>0.4</v>
-      </c>
       <c r="J8">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N8">
-        <v>0.2620238095238095</v>
+        <v>0.3097619047619048</v>
       </c>
       <c r="Q8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -932,37 +932,37 @@
         <v>40</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>0.05555555555555555</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>0.2620238095238095</v>
       </c>
       <c r="Q9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -1009,7 +1009,7 @@
         <v>0</v>
       </c>
       <c r="Q10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -1056,7 +1056,7 @@
         <v>0</v>
       </c>
       <c r="Q11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -1103,7 +1103,7 @@
         <v>0</v>
       </c>
       <c r="Q12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to scores for:
Wokingham
Greater London Authority
Cheshire West and Chester Council
South Tyneside Council
Luton Borough Council
</commit_message>
<xml_diff>
--- a/2021/combined_strategic_authorities.xlsx
+++ b/2021/combined_strategic_authorities.xlsx
@@ -650,7 +650,7 @@
         <v>34</v>
       </c>
       <c r="E3">
-        <v>0.4285714285714285</v>
+        <v>0.4761904761904762</v>
       </c>
       <c r="F3">
         <v>0.6666666666666666</v>
@@ -659,10 +659,10 @@
         <v>0.5714285714285714</v>
       </c>
       <c r="H3">
-        <v>0.7777777777777778</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="I3">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -677,7 +677,7 @@
         <v>0.75</v>
       </c>
       <c r="N3">
-        <v>0.6141666666666666</v>
+        <v>0.6579761904761904</v>
       </c>
       <c r="Q3" t="s">
         <v>45</v>

</xml_diff>